<commit_message>
tweaking numbers but need to figure out better way to throw away edges
</commit_message>
<xml_diff>
--- a/prog1/Book1.xlsx
+++ b/prog1/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="20115" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="20115" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,6 +212,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -233,42 +234,8 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.28947223636199471"/>
-                  <c:y val="-0.52493353993401426"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>y = 4.0351x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000"/>
-                      <a:t>-0.789</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>
-R² = 0.9999</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -333,42 +300,8 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.28755790293364814"/>
-                  <c:y val="-0.23711644478175167"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>y = 2.5661x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000"/>
-                      <a:t>-0.448</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>
-R² = 0.9833</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -433,42 +366,8 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.28564356950530156"/>
-                  <c:y val="4.6226691543075189E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>y = 1.6227x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000"/>
-                      <a:t>-0.268</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>
-R² = 0.9973</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -533,40 +432,20 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.28564356950530156"/>
-                  <c:y val="0.30135386691121441"/>
+                  <c:x val="0.27417213740293034"/>
+                  <c:y val="0.14742721537527018"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>y = 1.5783x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000"/>
-                      <a:t>-0.214</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>
-R² = 0.9907</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -628,11 +507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54783360"/>
-        <c:axId val="54801920"/>
+        <c:axId val="143000704"/>
+        <c:axId val="143002624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54783360"/>
+        <c:axId val="143000704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,18 +537,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54801920"/>
+        <c:crossAx val="143002624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54801920"/>
+        <c:axId val="143002624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,13 +577,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54783360"/>
+        <c:crossAx val="143000704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -730,8 +611,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85888543890163682"/>
-          <c:y val="0.16351178994191992"/>
+          <c:x val="0.82076352731493907"/>
+          <c:y val="0.15616934874642707"/>
           <c:w val="0.12962856052828367"/>
           <c:h val="0.65416774710390113"/>
         </c:manualLayout>
@@ -1312,11 +1193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54856704"/>
-        <c:axId val="54862976"/>
+        <c:axId val="149071360"/>
+        <c:axId val="149073280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54856704"/>
+        <c:axId val="149071360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,12 +1226,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54862976"/>
+        <c:crossAx val="149073280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54862976"/>
+        <c:axId val="149073280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1381,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54856704"/>
+        <c:crossAx val="149071360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1450,10 +1331,10 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1799,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>